<commit_message>
updated with user input prompt
</commit_message>
<xml_diff>
--- a/java_demo.xlsx
+++ b/java_demo.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>ID</t>
   </si>
@@ -23,34 +23,31 @@
     <t>LASTNAME</t>
   </si>
   <si>
-    <t>Amit</t>
+    <t>56</t>
   </si>
   <si>
-    <t>Shukla</t>
+    <t>hari ram</t>
   </si>
   <si>
-    <t>Lokesh</t>
+    <t>panchal</t>
   </si>
   <si>
-    <t>Gupta</t>
+    <t>78</t>
   </si>
   <si>
-    <t>John</t>
+    <t>mohan lal</t>
   </si>
   <si>
-    <t>Adwards</t>
+    <t>savita</t>
   </si>
   <si>
-    <t>Brian</t>
+    <t>dinesh sengar</t>
   </si>
   <si>
-    <t>Schultz</t>
+    <t>amra</t>
   </si>
   <si>
-    <t>Shiv</t>
-  </si>
-  <si>
-    <t>Bharadwaj</t>
+    <t/>
   </si>
 </sst>
 </file>
@@ -113,58 +110,36 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1.0</v>
+      <c r="A2" t="s">
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2.0</v>
+      <c r="A3" t="s">
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>3.0</v>
+      <c r="A4" t="s">
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="B6" t="s">
         <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>